<commit_message>
added description for all functions
</commit_message>
<xml_diff>
--- a/cahier_de_tests_calculatrice_Pierre.xlsx
+++ b/cahier_de_tests_calculatrice_Pierre.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierrot\Documents\HB_PharmaPilot\calculatrice\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierrot\Documents\HB_PharmaPilot\calculatrice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E551FCE3-3CEC-49B7-875A-E3903A4EEBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04038E16-DBAD-4BCE-97C2-0FB6D4BD20F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="17376" windowHeight="12336" activeTab="1" xr2:uid="{B44055BC-57CB-4C0A-99E7-8C611C2DB950}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B44055BC-57CB-4C0A-99E7-8C611C2DB950}"/>
   </bookViews>
   <sheets>
     <sheet name="Développeur" sheetId="1" r:id="rId1"/>
@@ -35,14 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="22">
   <si>
     <t>Scénario</t>
   </si>
   <si>
-    <t>Test de l'addition</t>
-  </si>
-  <si>
     <t>Input</t>
   </si>
   <si>
@@ -53,12 +50,6 @@
   </si>
   <si>
     <t>Etat</t>
-  </si>
-  <si>
-    <t>1 + 1</t>
-  </si>
-  <si>
-    <t>KO</t>
   </si>
   <si>
     <t>ok</t>
@@ -186,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -200,43 +191,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -255,28 +258,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B05828DD-E3D1-4EB7-9DB1-8789138CF034}" name="Tableau1" displayName="Tableau1" ref="A1:E2" totalsRowShown="0">
-  <autoFilter ref="A1:E2" xr:uid="{B05828DD-E3D1-4EB7-9DB1-8789138CF034}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B05828DD-E3D1-4EB7-9DB1-8789138CF034}" name="Tableau1" displayName="Tableau1" ref="A1:E11" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E11" xr:uid="{B05828DD-E3D1-4EB7-9DB1-8789138CF034}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{248BC16A-1685-488D-A22C-DE75AC3E58FC}" name="Scénario"/>
-    <tableColumn id="2" xr3:uid="{40BCA765-9860-46C1-82C7-382A196E91A0}" name="Input"/>
-    <tableColumn id="3" xr3:uid="{ABF3415F-136D-4AAE-902F-5C44E38562A5}" name="Résultat Attendu"/>
-    <tableColumn id="4" xr3:uid="{A8083F3B-B067-4073-812E-52901A31CED7}" name="Résultat Obtenu"/>
-    <tableColumn id="5" xr3:uid="{DAB24C2A-38EC-4F3F-B562-B3615DFA512A}" name="Etat"/>
+    <tableColumn id="1" xr3:uid="{248BC16A-1685-488D-A22C-DE75AC3E58FC}" name="Scénario" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{40BCA765-9860-46C1-82C7-382A196E91A0}" name="Input" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{ABF3415F-136D-4AAE-902F-5C44E38562A5}" name="Résultat Attendu" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{A8083F3B-B067-4073-812E-52901A31CED7}" name="Résultat Obtenu" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{DAB24C2A-38EC-4F3F-B562-B3615DFA512A}" name="Etat" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B46B2BCD-8D3F-47FF-A3FA-3C33A5E0E3DB}" name="Tableau2" displayName="Tableau2" ref="A1:E3" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E3" xr:uid="{B46B2BCD-8D3F-47FF-A3FA-3C33A5E0E3DB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B46B2BCD-8D3F-47FF-A3FA-3C33A5E0E3DB}" name="Tableau2" displayName="Tableau2" ref="A1:E11" totalsRowShown="0" dataDxfId="11">
+  <autoFilter ref="A1:E11" xr:uid="{B46B2BCD-8D3F-47FF-A3FA-3C33A5E0E3DB}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D3C7E472-F328-47CD-906E-6E4C73AD5204}" name="Scénario" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{E110DA5D-E52E-4425-9798-4F767A5554E8}" name="Input" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{81CD7CD5-47D1-419D-B9F8-AD3EDD50B6C8}" name="Résultat Attendu" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{58B3EBD3-2BED-4F59-9C5F-C0E4092418F5}" name="Résultat Obtenu" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{3704C978-7EA5-4464-9EB0-037966868566}" name="Etat" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D3C7E472-F328-47CD-906E-6E4C73AD5204}" name="Scénario" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{E110DA5D-E52E-4425-9798-4F767A5554E8}" name="Input" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{81CD7CD5-47D1-419D-B9F8-AD3EDD50B6C8}" name="Résultat Attendu" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{58B3EBD3-2BED-4F59-9C5F-C0E4092418F5}" name="Résultat Obtenu" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{3704C978-7EA5-4464-9EB0-037966868566}" name="Etat" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -579,17 +582,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE93CF6-8D21-4C19-9F9F-69A3082BF57C}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.88671875" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" customWidth="1"/>
     <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -599,33 +602,174 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="C4" s="3">
+        <v>100</v>
+      </c>
+      <c r="D4" s="3">
+        <v>100</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -641,7 +785,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,24 +802,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3">
         <v>11</v>
@@ -683,31 +827,27 @@
       <c r="D2" s="3">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3">
         <v>100</v>
@@ -719,25 +859,23 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3">
         <v>10</v>
@@ -745,88 +883,76 @@
       <c r="D6" s="3">
         <v>10</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>16</v>
+      <c r="A9" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>